<commit_message>
Replace verification with function AssertPreviewValue Fix .dyn files which has WriteTofile node and overwrite options true was required
</commit_message>
<xml_diff>
--- a/test/core/excel/Excel_MAGN7213_2.xlsx
+++ b/test/core/excel/Excel_MAGN7213_2.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8592" windowHeight="5604"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8592" windowHeight="5604" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet0" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId2"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -338,8 +340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -362,4 +364,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>